<commit_message>
nada sirve alv todo da error me quiero kys
</commit_message>
<xml_diff>
--- a/backend/aqui.xlsx
+++ b/backend/aqui.xlsx
@@ -25,247 +25,247 @@
     <t>108480432</t>
   </si>
   <si>
-    <t>isusana310</t>
+    <t>isusana481</t>
   </si>
   <si>
     <t>204500522</t>
   </si>
   <si>
-    <t>lelena425</t>
+    <t>lelena520</t>
   </si>
   <si>
     <t>205720051</t>
   </si>
   <si>
-    <t>jvargas255</t>
+    <t>jvargas250</t>
   </si>
   <si>
     <t>702180508</t>
   </si>
   <si>
-    <t>fchacón015</t>
+    <t>fchacón520</t>
   </si>
   <si>
     <t>205690746</t>
   </si>
   <si>
-    <t>avargas964</t>
+    <t>avargas546</t>
   </si>
   <si>
     <t>602160475</t>
   </si>
   <si>
-    <t>arojas247</t>
+    <t>arojas606</t>
   </si>
   <si>
     <t>109810603</t>
   </si>
   <si>
-    <t>cvargas101</t>
+    <t>cvargas910</t>
   </si>
   <si>
     <t>108780841</t>
   </si>
   <si>
-    <t>halpízar008</t>
+    <t>halpízar088</t>
   </si>
   <si>
     <t>602520067</t>
   </si>
   <si>
-    <t>rálvarez600</t>
+    <t>rálvarez670</t>
   </si>
   <si>
     <t>503360141</t>
   </si>
   <si>
-    <t>scamacho133</t>
+    <t>scamacho014</t>
   </si>
   <si>
     <t>203820981</t>
   </si>
   <si>
-    <t>hvíquez038</t>
+    <t>hvíquez221</t>
   </si>
   <si>
     <t>111190714</t>
   </si>
   <si>
-    <t>ppérez401</t>
+    <t>ppérez191</t>
   </si>
   <si>
     <t>208330983</t>
   </si>
   <si>
-    <t>augalde388</t>
+    <t>augalde080</t>
   </si>
   <si>
     <t>401240280</t>
   </si>
   <si>
-    <t>ccortés104</t>
+    <t>ccortés020</t>
   </si>
   <si>
     <t>111870703</t>
   </si>
   <si>
-    <t>lcastillo710</t>
+    <t>lcastillo300</t>
   </si>
   <si>
     <t>205240079</t>
   </si>
   <si>
-    <t>cdíaz924</t>
+    <t>cdíaz294</t>
   </si>
   <si>
     <t>109080164</t>
   </si>
   <si>
-    <t>yhernández106</t>
+    <t>yhernández601</t>
   </si>
   <si>
     <t>110410270</t>
   </si>
   <si>
-    <t>vsantos107</t>
+    <t>vsantos171</t>
   </si>
   <si>
     <t>401580258</t>
   </si>
   <si>
-    <t>gbarrantes020</t>
+    <t>gbarrantes885</t>
   </si>
   <si>
     <t>900990677</t>
   </si>
   <si>
-    <t>dálvarez670</t>
+    <t>dálvarez007</t>
   </si>
   <si>
     <t>204290474</t>
   </si>
   <si>
-    <t>vsegura440</t>
+    <t>vsegura020</t>
   </si>
   <si>
     <t>204160866</t>
   </si>
   <si>
-    <t>pcalvo006</t>
+    <t>pcalvo201</t>
   </si>
   <si>
     <t>205280759</t>
   </si>
   <si>
-    <t>yvargas722</t>
+    <t>yvargas925</t>
   </si>
   <si>
     <t>304770133</t>
   </si>
   <si>
-    <t>gsolano714</t>
+    <t>gsolano301</t>
   </si>
   <si>
     <t>204600069</t>
   </si>
   <si>
-    <t>omarín609</t>
+    <t>omarín460</t>
   </si>
   <si>
     <t>108170474</t>
   </si>
   <si>
-    <t>yabarca011</t>
+    <t>yabarca440</t>
   </si>
   <si>
     <t>205150149</t>
   </si>
   <si>
-    <t>mfallas590</t>
+    <t>mfallas490</t>
   </si>
   <si>
     <t>205310432</t>
   </si>
   <si>
-    <t>schavarría225</t>
+    <t>schavarría522</t>
   </si>
   <si>
     <t>801050664</t>
   </si>
   <si>
-    <t>asánchez056</t>
+    <t>asánchez641</t>
   </si>
   <si>
     <t>204660722</t>
   </si>
   <si>
-    <t>mzamora266</t>
+    <t>mzamora622</t>
   </si>
   <si>
     <t>112390952</t>
   </si>
   <si>
-    <t>abermúdez915</t>
+    <t>abermúdez019</t>
   </si>
   <si>
     <t>801220474</t>
   </si>
   <si>
-    <t>yhernández170</t>
+    <t>yhernández100</t>
   </si>
   <si>
     <t>205230399</t>
   </si>
   <si>
-    <t>lsalas903</t>
+    <t>lsalas339</t>
   </si>
   <si>
     <t>401430930</t>
   </si>
   <si>
-    <t>harce300</t>
+    <t>harce041</t>
   </si>
   <si>
     <t>206350665</t>
   </si>
   <si>
-    <t>marguello052</t>
+    <t>marguello265</t>
   </si>
   <si>
     <t>402170723</t>
   </si>
   <si>
-    <t>serasmo402</t>
+    <t>serasmo074</t>
   </si>
   <si>
     <t>206020735</t>
   </si>
   <si>
-    <t>agonzález026</t>
+    <t>agonzález230</t>
   </si>
   <si>
     <t>402160579</t>
   </si>
   <si>
-    <t>jmaría007</t>
+    <t>jmaría795</t>
   </si>
   <si>
     <t>110640818</t>
   </si>
   <si>
-    <t>cramírez086</t>
+    <t>cramírez181</t>
   </si>
   <si>
     <t>401770734</t>
   </si>
   <si>
-    <t>kbolaños443</t>
+    <t>kbolaños340</t>
   </si>
   <si>
     <t>207380463</t>
   </si>
   <si>
-    <t>cprado630</t>
+    <t>cprado320</t>
   </si>
   <si>
     <t>603650441</t>
@@ -277,73 +277,73 @@
     <t>401290471</t>
   </si>
   <si>
-    <t>fsánchez244</t>
+    <t>fsánchez400</t>
   </si>
   <si>
     <t>701960328</t>
   </si>
   <si>
-    <t>kvargas072</t>
+    <t>kvargas870</t>
   </si>
   <si>
     <t>207930528</t>
   </si>
   <si>
-    <t>mvalverde529</t>
+    <t>mvalverde872</t>
   </si>
   <si>
     <t>205270757</t>
   </si>
   <si>
-    <t>kcampos772</t>
+    <t>kcampos777</t>
   </si>
   <si>
     <t>205870017</t>
   </si>
   <si>
-    <t>ycórdoba578</t>
+    <t>ycórdoba257</t>
   </si>
   <si>
     <t>206260174</t>
   </si>
   <si>
-    <t>cyesenia274</t>
+    <t>cyesenia127</t>
   </si>
   <si>
     <t>110680456</t>
   </si>
   <si>
-    <t>ymaría451</t>
+    <t>ymaría614</t>
   </si>
   <si>
     <t>900960978</t>
   </si>
   <si>
-    <t>osegura679</t>
+    <t>osegura608</t>
   </si>
   <si>
     <t>603460661</t>
   </si>
   <si>
-    <t>rsoto636</t>
+    <t>rsoto066</t>
   </si>
   <si>
     <t>109660008</t>
   </si>
   <si>
-    <t>jcontreras918</t>
+    <t>jcontreras061</t>
   </si>
   <si>
     <t>108740930</t>
   </si>
   <si>
-    <t>macuña410</t>
+    <t>macuña000</t>
   </si>
   <si>
     <t>109620871</t>
   </si>
   <si>
-    <t>isalas201</t>
+    <t>isalas691</t>
   </si>
   <si>
     <t>204250440</t>
@@ -355,109 +355,109 @@
     <t>207580963</t>
   </si>
   <si>
-    <t>kbonilla729</t>
+    <t>kbonilla032</t>
   </si>
   <si>
     <t>205750300</t>
   </si>
   <si>
-    <t>gquesada750</t>
+    <t>gquesada753</t>
   </si>
   <si>
     <t>303960350</t>
   </si>
   <si>
-    <t>mcatalina009</t>
+    <t>mcatalina033</t>
   </si>
   <si>
     <t>207160153</t>
   </si>
   <si>
-    <t>jrodríguez160</t>
+    <t>jrodríguez162</t>
   </si>
   <si>
     <t>205360852</t>
   </si>
   <si>
-    <t>yruiz600</t>
+    <t>yruiz538</t>
   </si>
   <si>
     <t>204420924</t>
   </si>
   <si>
-    <t>rsalas229</t>
+    <t>rsalas240</t>
   </si>
   <si>
     <t>401750304</t>
   </si>
   <si>
-    <t>ecambronero514</t>
+    <t>ecambronero404</t>
   </si>
   <si>
     <t>113580076</t>
   </si>
   <si>
-    <t>mdenise031</t>
+    <t>mdenise675</t>
   </si>
   <si>
     <t>207280242</t>
   </si>
   <si>
-    <t>jsalazar422</t>
+    <t>jsalazar227</t>
   </si>
   <si>
     <t>105290664</t>
   </si>
   <si>
-    <t>alorena910</t>
+    <t>alorena066</t>
   </si>
   <si>
     <t>110580578</t>
   </si>
   <si>
-    <t>frojas817</t>
+    <t>frojas871</t>
   </si>
   <si>
     <t>206040198</t>
   </si>
   <si>
-    <t>karguedas924</t>
+    <t>karguedas689</t>
   </si>
   <si>
     <t>205780352</t>
   </si>
   <si>
-    <t>asalas385</t>
+    <t>asalas328</t>
   </si>
   <si>
     <t>603730502</t>
   </si>
   <si>
-    <t>bsteven305</t>
+    <t>bsteven562</t>
   </si>
   <si>
     <t>401750549</t>
   </si>
   <si>
-    <t>jarguedas090</t>
+    <t>jarguedas047</t>
   </si>
   <si>
     <t>800950490</t>
   </si>
   <si>
-    <t>despinoza080</t>
+    <t>despinoza095</t>
   </si>
   <si>
     <t>206600255</t>
   </si>
   <si>
-    <t>cquirós655</t>
+    <t>cquirós062</t>
   </si>
   <si>
     <t>107030870</t>
   </si>
   <si>
-    <t>jarturo001</t>
+    <t>jarturo773</t>
   </si>
   <si>
     <t>900890952</t>
@@ -469,175 +469,175 @@
     <t>114730519</t>
   </si>
   <si>
-    <t>fgonzález497</t>
+    <t>fgonzález715</t>
   </si>
   <si>
     <t>120850674</t>
   </si>
   <si>
-    <t>mgonzález725</t>
+    <t>mgonzález080</t>
   </si>
   <si>
     <t>205630892</t>
   </si>
   <si>
-    <t>hoviedo062</t>
+    <t>hoviedo895</t>
   </si>
   <si>
     <t>206330160</t>
   </si>
   <si>
-    <t>ycastillo003</t>
+    <t>ycastillo200</t>
   </si>
   <si>
     <t>504120071</t>
   </si>
   <si>
-    <t>kmiranda500</t>
+    <t>kmiranda410</t>
   </si>
   <si>
     <t>205950092</t>
   </si>
   <si>
-    <t>apalma025</t>
+    <t>apalma929</t>
   </si>
   <si>
     <t>303870965</t>
   </si>
   <si>
-    <t>rrojas659</t>
+    <t>rrojas576</t>
   </si>
   <si>
     <t>114140037</t>
   </si>
   <si>
-    <t>jazofeifa171</t>
+    <t>jazofeifa047</t>
   </si>
   <si>
     <t>401780847</t>
   </si>
   <si>
-    <t>pvargas078</t>
+    <t>pvargas778</t>
   </si>
   <si>
     <t>402040013</t>
   </si>
   <si>
-    <t>adíaz104</t>
+    <t>adíaz004</t>
   </si>
   <si>
     <t>205620142</t>
   </si>
   <si>
-    <t>hgamboa060</t>
+    <t>hgamboa201</t>
   </si>
   <si>
     <t>108890750</t>
   </si>
   <si>
-    <t>csolís958</t>
+    <t>csolís107</t>
   </si>
   <si>
     <t>206300145</t>
   </si>
   <si>
-    <t>jmurillo063</t>
+    <t>jmurillo305</t>
   </si>
   <si>
     <t>205910238</t>
   </si>
   <si>
-    <t>amaría803</t>
+    <t>amaría005</t>
   </si>
   <si>
     <t>603240688</t>
   </si>
   <si>
-    <t>equesada863</t>
+    <t>equesada868</t>
   </si>
   <si>
     <t>206750932</t>
   </si>
   <si>
-    <t>ggonzález053</t>
+    <t>ggonzález302</t>
   </si>
   <si>
     <t>603390980</t>
   </si>
   <si>
-    <t>jmanuel380</t>
+    <t>jmanuel893</t>
   </si>
   <si>
     <t>107400398</t>
   </si>
   <si>
-    <t>rmurillo719</t>
+    <t>rmurillo470</t>
   </si>
   <si>
     <t>108460513</t>
   </si>
   <si>
-    <t>kbryan863</t>
+    <t>kbryan084</t>
   </si>
   <si>
     <t>701830335</t>
   </si>
   <si>
-    <t>gbrenes753</t>
+    <t>gbrenes573</t>
   </si>
   <si>
     <t>110230935</t>
   </si>
   <si>
-    <t>gsoto231</t>
+    <t>gsoto125</t>
   </si>
   <si>
     <t>205540608</t>
   </si>
   <si>
-    <t>wrodríguez558</t>
+    <t>wrodríguez500</t>
   </si>
   <si>
     <t>701020697</t>
   </si>
   <si>
-    <t>mramírez702</t>
+    <t>mramírez170</t>
   </si>
   <si>
     <t>206490219</t>
   </si>
   <si>
-    <t>erodríguez920</t>
+    <t>erodríguez904</t>
   </si>
   <si>
     <t>603530302</t>
   </si>
   <si>
-    <t>koviedo530</t>
+    <t>koviedo306</t>
   </si>
   <si>
     <t>603440323</t>
   </si>
   <si>
-    <t>dvega330</t>
+    <t>dvega363</t>
   </si>
   <si>
     <t>401860636</t>
   </si>
   <si>
-    <t>abonilla146</t>
+    <t>abonilla166</t>
   </si>
   <si>
     <t>401990918</t>
   </si>
   <si>
-    <t>kjaen904</t>
+    <t>kjaen199</t>
   </si>
   <si>
     <t>401730295</t>
   </si>
   <si>
-    <t>mmagdalena203</t>
+    <t>mmagdalena905</t>
   </si>
 </sst>
 </file>

</xml_diff>